<commit_message>
Updated file is added
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LearnAutomationTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>firstname</t>
   </si>
@@ -36,6 +36,12 @@
   </si>
   <si>
     <t>Perma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alkesh </t>
+  </si>
+  <si>
+    <t>Rathore</t>
   </si>
 </sst>
 </file>
@@ -353,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,6 +383,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>